<commit_message>
Improved modem sleep mode. Fixed #8. Updated BOM.
</commit_message>
<xml_diff>
--- a/hw/BeeGl_Broker_Variant_A_BOM_rev1.0.xlsx
+++ b/hw/BeeGl_Broker_Variant_A_BOM_rev1.0.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="96">
   <si>
     <t>ID</t>
   </si>
@@ -298,6 +298,27 @@
   </si>
   <si>
     <t xml:space="preserve">Cut in  fragments to connect load cell with HX711 &amp; DHT22 case and DHT22 case with broker </t>
+  </si>
+  <si>
+    <t>M5x20 Hexagon socket Head Cap Screw</t>
+  </si>
+  <si>
+    <t>ISO 4762, A2 Stainless steel, Hexagon/Torx socket head cap screw, k=5mm, l=20mm
+http://www.fasteners.eu/standards/ISO/4762</t>
+  </si>
+  <si>
+    <t>M5x10 Hexagon socket Head Cap Screw</t>
+  </si>
+  <si>
+    <t>ISO 4762, A2  Stainless steel, Hexagon/Torx socket head cap screw, k=5mm, l=10mm
+http://www.fasteners.eu/standards/ISO/4762</t>
+  </si>
+  <si>
+    <t>M5 Hexagon Nut</t>
+  </si>
+  <si>
+    <t>ISO 4032, A2 Stainless steel Hexagon nut, m=~4.5, s=8
+http://www.fasteners.eu/standards/ISO/4032</t>
   </si>
 </sst>
 </file>
@@ -1251,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1537,76 +1558,70 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C15" s="4"/>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
         <v>37</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" ht="45">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" t="s">
         <v>37</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" ht="30">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E17" t="s">
         <v>37</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30">
+        <v>95</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="45">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="4"/>
+        <v>66</v>
+      </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>37</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45">
@@ -1614,7 +1629,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19">
@@ -1624,18 +1639,18 @@
         <v>37</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20">
@@ -1645,22 +1660,20 @@
         <v>37</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="45">
+    <row r="21" spans="1:7" ht="30">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
+      <c r="B21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="4"/>
       <c r="D21">
         <v>1</v>
       </c>
@@ -1668,24 +1681,31 @@
         <v>37</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30">
+        <v>40</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>62</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C22" s="4"/>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>63</v>
+        <v>42</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="45">
@@ -1693,8 +1713,9 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C23" s="4"/>
       <c r="D23">
         <v>1</v>
       </c>
@@ -1702,15 +1723,21 @@
         <v>37</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30">
+        <v>45</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>72</v>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1719,59 +1746,110 @@
         <v>37</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="135">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="4"/>
+        <v>62</v>
+      </c>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
         <v>37</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" ht="30">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="135">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" ht="30">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="C29" s="4"/>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="1"/>
+      <c r="G29" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="F3" r:id="rId2" display="https://www.sparkfun.com/products/13879_x000a_"/>
     <hyperlink ref="F4" r:id="rId3" display="https://www.aliexpress.com/wholesale?catId=0&amp;initiative_id=SB_20190705011301&amp;SearchText=battery+shield"/>
-    <hyperlink ref="F21" r:id="rId4" display="https://www.google.com/search?q=sim800l+v2.0"/>
+    <hyperlink ref="F24" r:id="rId4" display="https://www.google.com/search?q=sim800l+v2.0"/>
     <hyperlink ref="F5" r:id="rId5"/>
     <hyperlink ref="F6" r:id="rId6"/>
     <hyperlink ref="F8" r:id="rId7"/>
     <hyperlink ref="F12" r:id="rId8"/>
     <hyperlink ref="F13" r:id="rId9"/>
-    <hyperlink ref="F22" r:id="rId10"/>
+    <hyperlink ref="F25" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>